<commit_message>
AI, BL, BS, TG, UR
</commit_message>
<xml_diff>
--- a/AI_nais_einheiten_unique_mf.xlsx
+++ b/AI_nais_einheiten_unique_mf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frehnerm\Documents\excel\Aufträge\Sensi CH\Erledigt Abgabe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\develops\sensitivewaldstandorteCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F92B020-A1F8-4000-941B-47A4BC4941EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D85685-7D8F-4DC8-BCEF-0DFE70A2D7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="49035" yWindow="2490" windowWidth="19215" windowHeight="19530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2012" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2012" uniqueCount="309">
   <si>
     <t>WSTEinheit</t>
   </si>
@@ -941,6 +941,15 @@
   </si>
   <si>
     <t>hm(om)</t>
+  </si>
+  <si>
+    <t>nais</t>
+  </si>
+  <si>
+    <t>nais2</t>
+  </si>
+  <si>
+    <t>tahs</t>
   </si>
 </sst>
 </file>
@@ -1328,23 +1337,23 @@
   <dimension ref="A1:K291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K227" sqref="K227"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>301</v>
       </c>
@@ -1352,7 +1361,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>306</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1373,13 +1382,13 @@
         <v>1</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>2</v>
+        <v>307</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1399,7 +1408,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -1419,7 +1428,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>6</v>
       </c>
@@ -1439,7 +1448,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>8</v>
       </c>
@@ -1459,7 +1468,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>9</v>
       </c>
@@ -1479,7 +1488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>12</v>
       </c>
@@ -1499,7 +1508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>20</v>
       </c>
@@ -1519,7 +1528,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>23</v>
       </c>
@@ -1548,7 +1557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>27</v>
       </c>
@@ -1568,7 +1577,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>28</v>
       </c>
@@ -1597,7 +1606,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>29</v>
       </c>
@@ -1617,7 +1626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>31</v>
       </c>
@@ -1637,7 +1646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>32</v>
       </c>
@@ -1657,7 +1666,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>36</v>
       </c>
@@ -1677,7 +1686,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>39</v>
       </c>
@@ -1697,7 +1706,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>55</v>
       </c>
@@ -1726,7 +1735,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>61</v>
       </c>
@@ -1746,7 +1755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>62</v>
       </c>
@@ -1766,7 +1775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>64</v>
       </c>
@@ -1780,7 +1789,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>65</v>
       </c>
@@ -1800,7 +1809,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>66</v>
       </c>
@@ -1820,7 +1829,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>102</v>
       </c>
@@ -1840,7 +1849,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>113</v>
       </c>
@@ -1869,7 +1878,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>115</v>
       </c>
@@ -1892,7 +1901,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>120</v>
       </c>
@@ -1921,7 +1930,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>121</v>
       </c>
@@ -1941,7 +1950,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>122</v>
       </c>
@@ -1961,7 +1970,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>123</v>
       </c>
@@ -1990,7 +1999,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>124</v>
       </c>
@@ -2019,7 +2028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>144</v>
       </c>
@@ -2039,7 +2048,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>159</v>
       </c>
@@ -2068,7 +2077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>184</v>
       </c>
@@ -2088,7 +2097,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>185</v>
       </c>
@@ -2108,7 +2117,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>186</v>
       </c>
@@ -2128,7 +2137,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>191</v>
       </c>
@@ -2148,7 +2157,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>194</v>
       </c>
@@ -2168,7 +2177,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>203</v>
       </c>
@@ -2188,7 +2197,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>204</v>
       </c>
@@ -2217,7 +2226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>207</v>
       </c>
@@ -2246,7 +2255,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>212</v>
       </c>
@@ -2266,7 +2275,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>216</v>
       </c>
@@ -2286,7 +2295,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>217</v>
       </c>
@@ -2306,7 +2315,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>225</v>
       </c>
@@ -2335,7 +2344,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>226</v>
       </c>
@@ -2355,7 +2364,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>227</v>
       </c>
@@ -2375,7 +2384,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>240</v>
       </c>
@@ -2395,7 +2404,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>243</v>
       </c>
@@ -2424,7 +2433,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>247</v>
       </c>
@@ -2453,7 +2462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>254</v>
       </c>
@@ -2482,7 +2491,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>255</v>
       </c>
@@ -2511,7 +2520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>256</v>
       </c>
@@ -2540,7 +2549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>259</v>
       </c>
@@ -2569,7 +2578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>261</v>
       </c>
@@ -2598,7 +2607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>262</v>
       </c>
@@ -2627,7 +2636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>265</v>
       </c>
@@ -2647,7 +2656,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>275</v>
       </c>
@@ -2676,7 +2685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>279</v>
       </c>
@@ -2705,7 +2714,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>289</v>
       </c>
@@ -2734,7 +2743,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>293</v>
       </c>
@@ -2763,7 +2772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>342</v>
       </c>
@@ -2783,7 +2792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>348</v>
       </c>
@@ -2812,7 +2821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>351</v>
       </c>
@@ -2841,7 +2850,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>359</v>
       </c>
@@ -2870,7 +2879,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>395</v>
       </c>
@@ -2890,7 +2899,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>408</v>
       </c>
@@ -2919,7 +2928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>441</v>
       </c>
@@ -2948,7 +2957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>512</v>
       </c>
@@ -2977,7 +2986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>524</v>
       </c>
@@ -3006,7 +3015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>541</v>
       </c>
@@ -3026,7 +3035,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>563</v>
       </c>
@@ -3055,7 +3064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>608</v>
       </c>
@@ -3084,7 +3093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>717</v>
       </c>
@@ -3113,7 +3122,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>720</v>
       </c>
@@ -3142,7 +3151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>721</v>
       </c>
@@ -3162,7 +3171,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>724</v>
       </c>
@@ -3191,7 +3200,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>725</v>
       </c>
@@ -3211,7 +3220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>728</v>
       </c>
@@ -3240,7 +3249,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>732</v>
       </c>
@@ -3269,7 +3278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>740</v>
       </c>
@@ -3298,7 +3307,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>797</v>
       </c>
@@ -3318,7 +3327,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>802</v>
       </c>
@@ -3338,7 +3347,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>858</v>
       </c>
@@ -3367,7 +3376,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>869</v>
       </c>
@@ -3387,7 +3396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>873</v>
       </c>
@@ -3407,7 +3416,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>874</v>
       </c>
@@ -3436,7 +3445,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>885</v>
       </c>
@@ -3465,7 +3474,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>891</v>
       </c>
@@ -3494,7 +3503,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>898</v>
       </c>
@@ -3514,7 +3523,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>904</v>
       </c>
@@ -3534,7 +3543,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>928</v>
       </c>
@@ -3563,7 +3572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>957</v>
       </c>
@@ -3592,7 +3601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>1030</v>
       </c>
@@ -3621,7 +3630,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>1063</v>
       </c>
@@ -3650,7 +3659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>1097</v>
       </c>
@@ -3679,7 +3688,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>1148</v>
       </c>
@@ -3708,7 +3717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>1149</v>
       </c>
@@ -3737,7 +3746,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>1151</v>
       </c>
@@ -3766,7 +3775,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>1154</v>
       </c>
@@ -3795,7 +3804,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>1155</v>
       </c>
@@ -3824,7 +3833,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>1156</v>
       </c>
@@ -3853,7 +3862,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>1157</v>
       </c>
@@ -3882,7 +3891,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>1163</v>
       </c>
@@ -3911,7 +3920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>1164</v>
       </c>
@@ -3940,7 +3949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>1177</v>
       </c>
@@ -3969,7 +3978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>1179</v>
       </c>
@@ -3998,7 +4007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>1184</v>
       </c>
@@ -4027,7 +4036,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>1187</v>
       </c>
@@ -4056,7 +4065,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>1188</v>
       </c>
@@ -4085,7 +4094,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>1196</v>
       </c>
@@ -4114,7 +4123,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>1198</v>
       </c>
@@ -4143,7 +4152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>1200</v>
       </c>
@@ -4172,7 +4181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>1202</v>
       </c>
@@ -4201,7 +4210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>1215</v>
       </c>
@@ -4230,7 +4239,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>1218</v>
       </c>
@@ -4259,7 +4268,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>1230</v>
       </c>
@@ -4279,7 +4288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>1286</v>
       </c>
@@ -4308,7 +4317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>1292</v>
       </c>
@@ -4328,7 +4337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>1293</v>
       </c>
@@ -4357,7 +4366,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>1308</v>
       </c>
@@ -4377,7 +4386,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>1313</v>
       </c>
@@ -4397,7 +4406,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>1336</v>
       </c>
@@ -4417,7 +4426,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>1403</v>
       </c>
@@ -4446,7 +4455,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>1413</v>
       </c>
@@ -4475,7 +4484,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>1422</v>
       </c>
@@ -4504,7 +4513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>1584</v>
       </c>
@@ -4524,7 +4533,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>1628</v>
       </c>
@@ -4553,7 +4562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>1629</v>
       </c>
@@ -4582,7 +4591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>1631</v>
       </c>
@@ -4611,7 +4620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>1636</v>
       </c>
@@ -4640,7 +4649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>1640</v>
       </c>
@@ -4669,7 +4678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>1642</v>
       </c>
@@ -4698,7 +4707,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>1643</v>
       </c>
@@ -4727,7 +4736,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>1650</v>
       </c>
@@ -4756,7 +4765,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>1661</v>
       </c>
@@ -4776,7 +4785,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>1672</v>
       </c>
@@ -4805,7 +4814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>1673</v>
       </c>
@@ -4825,7 +4834,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>1674</v>
       </c>
@@ -4854,7 +4863,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>1675</v>
       </c>
@@ -4883,7 +4892,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>1688</v>
       </c>
@@ -4912,7 +4921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>1706</v>
       </c>
@@ -4941,7 +4950,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>1708</v>
       </c>
@@ -4970,7 +4979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>1710</v>
       </c>
@@ -4990,7 +4999,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>1725</v>
       </c>
@@ -5010,7 +5019,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>1733</v>
       </c>
@@ -5030,7 +5039,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>1754</v>
       </c>
@@ -5050,7 +5059,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>1823</v>
       </c>
@@ -5079,7 +5088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>1835</v>
       </c>
@@ -5108,7 +5117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>1862</v>
       </c>
@@ -5137,7 +5146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>1923</v>
       </c>
@@ -5166,7 +5175,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>1981</v>
       </c>
@@ -5195,7 +5204,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>1989</v>
       </c>
@@ -5224,7 +5233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>1993</v>
       </c>
@@ -5253,7 +5262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>1999</v>
       </c>
@@ -5282,7 +5291,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>2003</v>
       </c>
@@ -5311,7 +5320,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>2019</v>
       </c>
@@ -5340,7 +5349,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>2021</v>
       </c>
@@ -5369,7 +5378,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>2031</v>
       </c>
@@ -5392,7 +5401,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>2069</v>
       </c>
@@ -5412,7 +5421,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>2077</v>
       </c>
@@ -5441,7 +5450,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>2079</v>
       </c>
@@ -5461,7 +5470,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>2109</v>
       </c>
@@ -5490,7 +5499,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>2110</v>
       </c>
@@ -5519,7 +5528,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>2111</v>
       </c>
@@ -5548,7 +5557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>2136</v>
       </c>
@@ -5568,7 +5577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>2151</v>
       </c>
@@ -5588,7 +5597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>2153</v>
       </c>
@@ -5617,7 +5626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>2174</v>
       </c>
@@ -5646,7 +5655,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>2175</v>
       </c>
@@ -5675,7 +5684,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>2178</v>
       </c>
@@ -5704,7 +5713,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>2182</v>
       </c>
@@ -5733,7 +5742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>2191</v>
       </c>
@@ -5762,7 +5771,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>2199</v>
       </c>
@@ -5791,7 +5800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>2212</v>
       </c>
@@ -5811,7 +5820,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>2222</v>
       </c>
@@ -5840,7 +5849,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>2239</v>
       </c>
@@ -5860,7 +5869,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>2241</v>
       </c>
@@ -5880,7 +5889,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>2249</v>
       </c>
@@ -5900,7 +5909,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>2250</v>
       </c>
@@ -5929,7 +5938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>2252</v>
       </c>
@@ -5958,7 +5967,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>2264</v>
       </c>
@@ -5987,7 +5996,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>2292</v>
       </c>
@@ -6016,7 +6025,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>2293</v>
       </c>
@@ -6045,7 +6054,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>2300</v>
       </c>
@@ -6074,7 +6083,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>2313</v>
       </c>
@@ -6103,7 +6112,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>2314</v>
       </c>
@@ -6132,7 +6141,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>2315</v>
       </c>
@@ -6161,7 +6170,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>2316</v>
       </c>
@@ -6181,7 +6190,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>2317</v>
       </c>
@@ -6201,7 +6210,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>2344</v>
       </c>
@@ -6221,7 +6230,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>2348</v>
       </c>
@@ -6241,7 +6250,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>2349</v>
       </c>
@@ -6261,7 +6270,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>2350</v>
       </c>
@@ -6281,7 +6290,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>2351</v>
       </c>
@@ -6301,7 +6310,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>2352</v>
       </c>
@@ -6321,7 +6330,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>2355</v>
       </c>
@@ -6341,7 +6350,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>2360</v>
       </c>
@@ -6370,7 +6379,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>2363</v>
       </c>
@@ -6390,7 +6399,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>2366</v>
       </c>
@@ -6410,7 +6419,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>2372</v>
       </c>
@@ -6430,7 +6439,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>2373</v>
       </c>
@@ -6459,7 +6468,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>2382</v>
       </c>
@@ -6488,7 +6497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>2391</v>
       </c>
@@ -6508,7 +6517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>2392</v>
       </c>
@@ -6537,7 +6546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>2436</v>
       </c>
@@ -6566,7 +6575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>2446</v>
       </c>
@@ -6586,7 +6595,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>2470</v>
       </c>
@@ -6615,7 +6624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>2474</v>
       </c>
@@ -6644,7 +6653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>2479</v>
       </c>
@@ -6673,7 +6682,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>2482</v>
       </c>
@@ -6702,7 +6711,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>2484</v>
       </c>
@@ -6731,7 +6740,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>2497</v>
       </c>
@@ -6751,7 +6760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>2499</v>
       </c>
@@ -6771,7 +6780,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>2500</v>
       </c>
@@ -6791,7 +6800,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>2508</v>
       </c>
@@ -6820,7 +6829,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>2515</v>
       </c>
@@ -6849,7 +6858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>2538</v>
       </c>
@@ -6878,7 +6887,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>2543</v>
       </c>
@@ -6904,7 +6913,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>2565</v>
       </c>
@@ -6933,7 +6942,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>2598</v>
       </c>
@@ -6962,7 +6971,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>2601</v>
       </c>
@@ -6991,7 +7000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>2734</v>
       </c>
@@ -7017,7 +7026,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>2783</v>
       </c>
@@ -7046,7 +7055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>2786</v>
       </c>
@@ -7075,7 +7084,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>2792</v>
       </c>
@@ -7104,7 +7113,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>2797</v>
       </c>
@@ -7133,7 +7142,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>2976</v>
       </c>
@@ -7162,7 +7171,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>2981</v>
       </c>
@@ -7182,7 +7191,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>3083</v>
       </c>
@@ -7211,7 +7220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>3131</v>
       </c>
@@ -7240,7 +7249,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>3303</v>
       </c>
@@ -7269,7 +7278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>3323</v>
       </c>
@@ -7289,7 +7298,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>3434</v>
       </c>
@@ -7309,7 +7318,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>3437</v>
       </c>
@@ -7338,7 +7347,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>3442</v>
       </c>
@@ -7367,7 +7376,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>3446</v>
       </c>
@@ -7396,7 +7405,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>3457</v>
       </c>
@@ -7425,7 +7434,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>3469</v>
       </c>
@@ -7445,7 +7454,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>3474</v>
       </c>
@@ -7474,7 +7483,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>3493</v>
       </c>
@@ -7503,7 +7512,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>3506</v>
       </c>
@@ -7523,7 +7532,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>3623</v>
       </c>
@@ -7549,7 +7558,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>3643</v>
       </c>
@@ -7569,7 +7578,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>3645</v>
       </c>
@@ -7589,7 +7598,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>3651</v>
       </c>
@@ -7609,7 +7618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>3674</v>
       </c>
@@ -7638,7 +7647,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>3683</v>
       </c>
@@ -7667,7 +7676,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>3708</v>
       </c>
@@ -7696,7 +7705,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>3743</v>
       </c>
@@ -7725,7 +7734,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>3757</v>
       </c>
@@ -7745,7 +7754,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>3758</v>
       </c>
@@ -7765,7 +7774,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>3830</v>
       </c>
@@ -7794,7 +7803,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>3857</v>
       </c>
@@ -7823,7 +7832,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>3906</v>
       </c>
@@ -7852,7 +7861,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>3934</v>
       </c>
@@ -7881,7 +7890,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>3967</v>
       </c>
@@ -7907,7 +7916,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>3987</v>
       </c>
@@ -7927,7 +7936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>4002</v>
       </c>
@@ -7947,7 +7956,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>4020</v>
       </c>
@@ -7967,7 +7976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>4031</v>
       </c>
@@ -7996,7 +8005,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>4036</v>
       </c>
@@ -8025,7 +8034,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>4071</v>
       </c>
@@ -8054,7 +8063,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>4116</v>
       </c>
@@ -8083,7 +8092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>4134</v>
       </c>
@@ -8112,7 +8121,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>4135</v>
       </c>
@@ -8138,7 +8147,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>4167</v>
       </c>
@@ -8167,7 +8176,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>4253</v>
       </c>
@@ -8187,7 +8196,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>4259</v>
       </c>
@@ -8207,7 +8216,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>4260</v>
       </c>
@@ -8236,7 +8245,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>4264</v>
       </c>
@@ -8265,7 +8274,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>4305</v>
       </c>
@@ -8294,7 +8303,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>4349</v>
       </c>
@@ -8323,7 +8332,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>4359</v>
       </c>
@@ -8352,7 +8361,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>4360</v>
       </c>
@@ -8381,7 +8390,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>4368</v>
       </c>
@@ -8410,7 +8419,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>4528</v>
       </c>
@@ -8436,7 +8445,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>4873</v>
       </c>
@@ -8465,7 +8474,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>4875</v>
       </c>
@@ -8494,7 +8503,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>4907</v>
       </c>
@@ -8523,7 +8532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>4918</v>
       </c>
@@ -8552,7 +8561,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>4919</v>
       </c>
@@ -8581,7 +8590,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>5226</v>
       </c>
@@ -8610,7 +8619,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>5310</v>
       </c>
@@ -8636,7 +8645,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>5311</v>
       </c>
@@ -8665,7 +8674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>5399</v>
       </c>
@@ -8685,7 +8694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>5461</v>
       </c>
@@ -8714,7 +8723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>5469</v>
       </c>
@@ -8743,7 +8752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>5552</v>
       </c>
@@ -8772,7 +8781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>5674</v>
       </c>
@@ -8786,7 +8795,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>5730</v>
       </c>
@@ -8815,7 +8824,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>5744</v>
       </c>
@@ -8845,7 +8854,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:K291" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>